<commit_message>
See detailed descrition for changes in matrix
Added columns: 
- vSRD_TNKR
- vSRD_RCVR
- max_as_M

changed column name: max_as to max_as_KCAS

- Deleted all USA KC-10 aircraft (because USA does not have them anymore)
- Filled in missing data from Australia
- Added MMF Tanker with receivers: B-1B, B-2A, F-16A/B/C/D/E, F-35A/B/C.

Next step: MMF tanker with receiver: F-22, C-17, B-52
</commit_message>
<xml_diff>
--- a/Database/AAR_matrix.xlsx
+++ b/Database/AAR_matrix.xlsx
@@ -3267,8 +3267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q94" sqref="Q94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6412,6 +6412,9 @@
       <c r="O58">
         <v>325</v>
       </c>
+      <c r="P58">
+        <v>0.85</v>
+      </c>
       <c r="Q58">
         <f t="shared" si="4"/>
         <v>2425.0819999999999</v>
@@ -6463,6 +6466,9 @@
       <c r="O59">
         <v>325</v>
       </c>
+      <c r="P59">
+        <v>0.85</v>
+      </c>
       <c r="Q59">
         <f t="shared" si="4"/>
         <v>2425.0819999999999</v>
@@ -6514,6 +6520,9 @@
       <c r="O60">
         <v>325</v>
       </c>
+      <c r="P60">
+        <v>0.85</v>
+      </c>
       <c r="Q60">
         <f t="shared" si="4"/>
         <v>2425.0819999999999</v>
@@ -6565,6 +6574,9 @@
       <c r="O61">
         <v>325</v>
       </c>
+      <c r="P61">
+        <v>0.85</v>
+      </c>
       <c r="Q61">
         <f t="shared" si="4"/>
         <v>2425.0819999999999</v>
@@ -6616,6 +6628,9 @@
       <c r="O62">
         <v>300</v>
       </c>
+      <c r="P62">
+        <v>0.86</v>
+      </c>
       <c r="Q62">
         <f>900*2.20462</f>
         <v>1984.1579999999999</v>
@@ -6667,6 +6682,9 @@
       <c r="O63">
         <v>300</v>
       </c>
+      <c r="P63">
+        <v>0.86</v>
+      </c>
       <c r="Q63">
         <f t="shared" ref="Q63:Q67" si="5">900*2.20462</f>
         <v>1984.1579999999999</v>
@@ -6718,6 +6736,9 @@
       <c r="O64">
         <v>300</v>
       </c>
+      <c r="P64">
+        <v>0.86</v>
+      </c>
       <c r="Q64">
         <f t="shared" si="5"/>
         <v>1984.1579999999999</v>
@@ -6769,6 +6790,9 @@
       <c r="O65">
         <v>300</v>
       </c>
+      <c r="P65">
+        <v>0.86</v>
+      </c>
       <c r="Q65">
         <f t="shared" si="5"/>
         <v>1984.1579999999999</v>
@@ -6820,6 +6844,9 @@
       <c r="O66">
         <v>300</v>
       </c>
+      <c r="P66">
+        <v>0.86</v>
+      </c>
       <c r="Q66">
         <f t="shared" si="5"/>
         <v>1984.1579999999999</v>
@@ -6871,6 +6898,9 @@
       <c r="O67">
         <v>300</v>
       </c>
+      <c r="P67">
+        <v>0.86</v>
+      </c>
       <c r="Q67">
         <f t="shared" si="5"/>
         <v>1984.1579999999999</v>
@@ -6922,6 +6952,9 @@
       <c r="O68">
         <v>325</v>
       </c>
+      <c r="P68">
+        <v>0.86</v>
+      </c>
       <c r="Q68">
         <f>890*2.20462</f>
         <v>1962.1117999999999</v>
@@ -6973,6 +7006,9 @@
       <c r="O69">
         <v>325</v>
       </c>
+      <c r="P69">
+        <v>0.86</v>
+      </c>
       <c r="Q69">
         <f t="shared" ref="Q69:Q71" si="6">890*2.20462</f>
         <v>1962.1117999999999</v>
@@ -7024,6 +7060,9 @@
       <c r="O70">
         <v>325</v>
       </c>
+      <c r="P70">
+        <v>0.86</v>
+      </c>
       <c r="Q70">
         <f t="shared" si="6"/>
         <v>1962.1117999999999</v>
@@ -7075,6 +7114,9 @@
       <c r="O71">
         <v>325</v>
       </c>
+      <c r="P71">
+        <v>0.86</v>
+      </c>
       <c r="Q71">
         <f t="shared" si="6"/>
         <v>1962.1117999999999</v>
@@ -7126,6 +7168,9 @@
       <c r="O72">
         <v>325</v>
       </c>
+      <c r="P72">
+        <v>0.86</v>
+      </c>
       <c r="Q72">
         <f>1100*2.20462</f>
         <v>2425.0819999999999</v>
@@ -7177,6 +7222,9 @@
       <c r="O73">
         <v>325</v>
       </c>
+      <c r="P73">
+        <v>0.86</v>
+      </c>
       <c r="Q73">
         <f t="shared" ref="Q73:Q76" si="7">1100*2.20462</f>
         <v>2425.0819999999999</v>
@@ -7228,6 +7276,9 @@
       <c r="O74">
         <v>325</v>
       </c>
+      <c r="P74">
+        <v>0.86</v>
+      </c>
       <c r="Q74">
         <f t="shared" si="7"/>
         <v>2425.0819999999999</v>
@@ -7279,6 +7330,9 @@
       <c r="O75">
         <v>325</v>
       </c>
+      <c r="P75">
+        <v>0.86</v>
+      </c>
       <c r="Q75">
         <f t="shared" si="7"/>
         <v>2425.0819999999999</v>
@@ -7330,6 +7384,9 @@
       <c r="O76">
         <v>325</v>
       </c>
+      <c r="P76">
+        <v>0.86</v>
+      </c>
       <c r="Q76">
         <f t="shared" si="7"/>
         <v>2425.0819999999999</v>
@@ -7381,6 +7438,9 @@
       <c r="O77">
         <v>300</v>
       </c>
+      <c r="P77">
+        <v>0.86</v>
+      </c>
       <c r="Q77">
         <f>900*2.20462</f>
         <v>1984.1579999999999</v>
@@ -7431,6 +7491,9 @@
       </c>
       <c r="O78">
         <v>300</v>
+      </c>
+      <c r="P78">
+        <v>0.86</v>
       </c>
       <c r="Q78">
         <f>900*2.20462</f>
@@ -14601,7 +14664,7 @@
       <formula>COUNTIFS($A:$A,$A2,$B:$B,$B2,$C:$C,$C2,$D:$D,$D2,$E:$E,$E2,$F:$F,$F2)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B34 D51:I55 A49:C62 A139:F144 A103:F136 G103:H144 G45:Q46 D56:H57 A79:I79 G47:I55 A45:F48 D49:F50 A171:Q242 I56:I78 A58:H78 A80:H102 A30:Q44 A145:H170 J47:Q170 I80:I170">
+  <conditionalFormatting sqref="B2:B34 D51:I55 A49:C62 A139:F144 A103:F136 G103:H144 G45:Q46 D56:H57 A79:I79 G47:I55 A45:F48 D49:F50 A171:Q242 I56:I78 A58:H78 A80:H102 A30:Q44 A145:H170 I80:I170 J47:Q170">
     <cfRule type="containsBlanks" dxfId="98" priority="151">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
@@ -14626,7 +14689,7 @@
       <formula>COUNTIFS($A:$A,$A13,$B:$B,#REF!,$C:$C,#REF!,$D:$D,$D13,$E:$E,$E11,$F:$F,$F11)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51:I55 A49:C62 A139:F144 A103:F136 G103:H144 D56:H57 A79:I79 G47:I50 G45:R46 A45:F48 D49:F50 A171:R766 I47:R78 A58:H78 A80:H102 A2:R44 A145:H170 J79:R170 I80:I170">
+  <conditionalFormatting sqref="D51:I55 A49:C62 A139:F144 A103:F136 G103:H144 D56:H57 A79:I79 G47:I50 G45:R46 A45:F48 D49:F50 A171:R766 A58:H78 A80:H102 A2:R44 A145:H170 J79:R170 I80:I170 I47:R78">
     <cfRule type="containsText" dxfId="93" priority="150" operator="containsText" text="itv">
       <formula>NOT(ISERROR(SEARCH("itv",A2)))</formula>
     </cfRule>

</xml_diff>